<commit_message>
Seance du 15 fevrier 2019
</commit_message>
<xml_diff>
--- a/Gantt final.xlsx
+++ b/Gantt final.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E77671-DB99-41CF-A04B-BB8AB0C9866C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6DDA95-1E94-424E-A71E-EF20E6FAF537}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>Créez un diagramme de Gantt dans cette feuille de calcul.
 Entrez le titre de ce projet dans la cellule B1. 
@@ -134,15 +134,6 @@
     <t>Pisitionnement GPS</t>
   </si>
   <si>
-    <t>Stabilisation par flux video</t>
-  </si>
-  <si>
-    <t>Phase atterissage</t>
-  </si>
-  <si>
-    <t>Modbus master</t>
-  </si>
-  <si>
     <t>Feu de signalisation</t>
   </si>
   <si>
@@ -153,9 +144,6 @@
   </si>
   <si>
     <t>Contrôles électroaimants</t>
-  </si>
-  <si>
-    <t>Modbus slave</t>
   </si>
   <si>
     <t>Contrôle orientation cellules</t>
@@ -173,9 +161,6 @@
     <t>Asservissement de la base</t>
   </si>
   <si>
-    <t>Liaison des modules</t>
-  </si>
-  <si>
     <t>Vincent HONNORATY</t>
   </si>
   <si>
@@ -186,6 +171,24 @@
   </si>
   <si>
     <t>PROJET DRONE</t>
+  </si>
+  <si>
+    <t>Modbus master/slave</t>
+  </si>
+  <si>
+    <t>*Stabilisation par flux video</t>
+  </si>
+  <si>
+    <t>*Phase atterissage</t>
+  </si>
+  <si>
+    <t>Groupe (option)</t>
+  </si>
+  <si>
+    <t>Options</t>
+  </si>
+  <si>
+    <t>Interfaces avec l'extérieur</t>
   </si>
 </sst>
 </file>
@@ -1505,7 +1508,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="39" fmlaLink="$E$3" horiz="1" max="365" page="0" val="20"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="39" fmlaLink="$E$3" horiz="1" max="365" page="0" val="42"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1564,8 +1567,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{70B51325-D3C3-4A05-BAB3-7A7400707A14}" name="Jalons" displayName="Jalons" ref="B6:F25" totalsRowShown="0">
-  <autoFilter ref="B6:F25" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{70B51325-D3C3-4A05-BAB3-7A7400707A14}" name="Jalons" displayName="Jalons" ref="B6:F23" totalsRowShown="0">
+  <autoFilter ref="B6:F23" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1854,10 +1857,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BN40"/>
+  <dimension ref="A1:BN37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B2" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="AK3" sqref="AK3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1878,7 +1881,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1"/>
       <c r="E1"/>
@@ -1917,7 +1920,7 @@
       </c>
       <c r="D3" s="64"/>
       <c r="E3" s="31">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="H3" s="38"/>
       <c r="I3" s="39"/>
@@ -1943,7 +1946,7 @@
       </c>
       <c r="H4" s="13" t="str">
         <f ca="1">TEXT(H5,"mmmm")</f>
-        <v>février</v>
+        <v>mars</v>
       </c>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
@@ -1953,7 +1956,7 @@
       <c r="N4" s="13"/>
       <c r="O4" s="13" t="str">
         <f ca="1">IF(TEXT(O5,"mmmm")=H4,"",TEXT(O5,"mmmm"))</f>
-        <v>mars</v>
+        <v/>
       </c>
       <c r="P4" s="13"/>
       <c r="Q4" s="13"/>
@@ -1963,7 +1966,7 @@
       <c r="U4" s="13"/>
       <c r="V4" s="13" t="str">
         <f ca="1">IF(OR(TEXT(V5,"mmmm")=O4,TEXT(V5,"mmmm")=H4),"",TEXT(V5,"mmmm"))</f>
-        <v/>
+        <v>avril</v>
       </c>
       <c r="W4" s="13"/>
       <c r="X4" s="13"/>
@@ -1993,7 +1996,7 @@
       <c r="AP4" s="13"/>
       <c r="AQ4" s="13" t="str">
         <f ca="1">IF(OR(TEXT(AQ5,"mmmm")=AJ4,TEXT(AQ5,"mmmm")=AC4,TEXT(AQ5,"mmmm")=V4,TEXT(AQ5,"mmmm")=O4),"",TEXT(AQ5,"mmmm"))</f>
-        <v>avril</v>
+        <v/>
       </c>
       <c r="AR4" s="13"/>
       <c r="AS4" s="13"/>
@@ -2003,7 +2006,7 @@
       <c r="AW4" s="13"/>
       <c r="AX4" s="13" t="str">
         <f ca="1">IF(OR(TEXT(AX5,"mmmm")=AQ4,TEXT(AX5,"mmmm")=AJ4,TEXT(AX5,"mmmm")=AC4,TEXT(AX5,"mmmm")=V4),"",TEXT(AX5,"mmmm"))</f>
-        <v/>
+        <v>mai</v>
       </c>
       <c r="AY4" s="13"/>
       <c r="AZ4" s="13"/>
@@ -2030,227 +2033,227 @@
       <c r="G5" s="27"/>
       <c r="H5" s="41">
         <f ca="1">IFERROR(Début_Projet+Incrément_Défilement,TODAY())</f>
-        <v>43524</v>
+        <v>43546</v>
       </c>
       <c r="I5" s="42">
         <f ca="1">H5+1</f>
-        <v>43525</v>
+        <v>43547</v>
       </c>
       <c r="J5" s="43">
         <f t="shared" ref="J5:AW5" ca="1" si="0">I5+1</f>
-        <v>43526</v>
+        <v>43548</v>
       </c>
       <c r="K5" s="43">
         <f ca="1">J5+1</f>
-        <v>43527</v>
+        <v>43549</v>
       </c>
       <c r="L5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43528</v>
+        <v>43550</v>
       </c>
       <c r="M5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43529</v>
+        <v>43551</v>
       </c>
       <c r="N5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43530</v>
+        <v>43552</v>
       </c>
       <c r="O5" s="43">
         <f ca="1">N5+1</f>
-        <v>43531</v>
+        <v>43553</v>
       </c>
       <c r="P5" s="43">
         <f ca="1">O5+1</f>
-        <v>43532</v>
+        <v>43554</v>
       </c>
       <c r="Q5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43533</v>
+        <v>43555</v>
       </c>
       <c r="R5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43534</v>
+        <v>43556</v>
       </c>
       <c r="S5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43535</v>
+        <v>43557</v>
       </c>
       <c r="T5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43536</v>
+        <v>43558</v>
       </c>
       <c r="U5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43537</v>
+        <v>43559</v>
       </c>
       <c r="V5" s="43">
         <f ca="1">U5+1</f>
-        <v>43538</v>
+        <v>43560</v>
       </c>
       <c r="W5" s="43">
         <f ca="1">V5+1</f>
-        <v>43539</v>
+        <v>43561</v>
       </c>
       <c r="X5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43540</v>
+        <v>43562</v>
       </c>
       <c r="Y5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43541</v>
+        <v>43563</v>
       </c>
       <c r="Z5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43542</v>
+        <v>43564</v>
       </c>
       <c r="AA5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43543</v>
+        <v>43565</v>
       </c>
       <c r="AB5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43544</v>
+        <v>43566</v>
       </c>
       <c r="AC5" s="43">
         <f ca="1">AB5+1</f>
-        <v>43545</v>
+        <v>43567</v>
       </c>
       <c r="AD5" s="43">
         <f ca="1">AC5+1</f>
-        <v>43546</v>
+        <v>43568</v>
       </c>
       <c r="AE5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43547</v>
+        <v>43569</v>
       </c>
       <c r="AF5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43548</v>
+        <v>43570</v>
       </c>
       <c r="AG5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43549</v>
+        <v>43571</v>
       </c>
       <c r="AH5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43550</v>
+        <v>43572</v>
       </c>
       <c r="AI5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43551</v>
+        <v>43573</v>
       </c>
       <c r="AJ5" s="43">
         <f ca="1">AI5+1</f>
-        <v>43552</v>
+        <v>43574</v>
       </c>
       <c r="AK5" s="43">
         <f ca="1">AJ5+1</f>
-        <v>43553</v>
+        <v>43575</v>
       </c>
       <c r="AL5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43554</v>
+        <v>43576</v>
       </c>
       <c r="AM5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43555</v>
+        <v>43577</v>
       </c>
       <c r="AN5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43556</v>
+        <v>43578</v>
       </c>
       <c r="AO5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43557</v>
+        <v>43579</v>
       </c>
       <c r="AP5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43558</v>
+        <v>43580</v>
       </c>
       <c r="AQ5" s="43">
         <f ca="1">AP5+1</f>
-        <v>43559</v>
+        <v>43581</v>
       </c>
       <c r="AR5" s="43">
         <f ca="1">AQ5+1</f>
-        <v>43560</v>
+        <v>43582</v>
       </c>
       <c r="AS5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43561</v>
+        <v>43583</v>
       </c>
       <c r="AT5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43562</v>
+        <v>43584</v>
       </c>
       <c r="AU5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43563</v>
+        <v>43585</v>
       </c>
       <c r="AV5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43564</v>
+        <v>43586</v>
       </c>
       <c r="AW5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>43565</v>
+        <v>43587</v>
       </c>
       <c r="AX5" s="43">
         <f t="shared" ref="AX5:BK5" ca="1" si="1">AW5+1</f>
-        <v>43566</v>
+        <v>43588</v>
       </c>
       <c r="AY5" s="43">
         <f t="shared" ca="1" si="1"/>
-        <v>43567</v>
+        <v>43589</v>
       </c>
       <c r="AZ5" s="43">
         <f t="shared" ca="1" si="1"/>
-        <v>43568</v>
+        <v>43590</v>
       </c>
       <c r="BA5" s="43">
         <f t="shared" ca="1" si="1"/>
-        <v>43569</v>
+        <v>43591</v>
       </c>
       <c r="BB5" s="43">
         <f t="shared" ca="1" si="1"/>
-        <v>43570</v>
+        <v>43592</v>
       </c>
       <c r="BC5" s="43">
         <f t="shared" ca="1" si="1"/>
-        <v>43571</v>
+        <v>43593</v>
       </c>
       <c r="BD5" s="43">
         <f t="shared" ca="1" si="1"/>
-        <v>43572</v>
+        <v>43594</v>
       </c>
       <c r="BE5" s="43">
         <f t="shared" ca="1" si="1"/>
-        <v>43573</v>
+        <v>43595</v>
       </c>
       <c r="BF5" s="43">
         <f t="shared" ca="1" si="1"/>
-        <v>43574</v>
+        <v>43596</v>
       </c>
       <c r="BG5" s="43">
         <f t="shared" ca="1" si="1"/>
-        <v>43575</v>
+        <v>43597</v>
       </c>
       <c r="BH5" s="43">
         <f t="shared" ca="1" si="1"/>
-        <v>43576</v>
+        <v>43598</v>
       </c>
       <c r="BI5" s="43">
         <f t="shared" ca="1" si="1"/>
-        <v>43577</v>
+        <v>43599</v>
       </c>
       <c r="BJ5" s="43">
         <f t="shared" ca="1" si="1"/>
-        <v>43578</v>
+        <v>43600</v>
       </c>
       <c r="BK5" s="44">
         <f t="shared" ca="1" si="1"/>
-        <v>43579</v>
+        <v>43601</v>
       </c>
     </row>
     <row r="6" spans="1:63" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2279,19 +2282,19 @@
       </c>
       <c r="I6" s="35" t="str">
         <f t="shared" ref="I6:AM6" ca="1" si="2">LEFT(TEXT(I5,"jjj"),1)</f>
-        <v>v</v>
+        <v>s</v>
       </c>
       <c r="J6" s="37" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="K6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>d</v>
+        <v>l</v>
       </c>
       <c r="L6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>l</v>
+        <v>m</v>
       </c>
       <c r="M6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -2299,27 +2302,27 @@
       </c>
       <c r="N6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>m</v>
+        <v>j</v>
       </c>
       <c r="O6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>j</v>
+        <v>v</v>
       </c>
       <c r="P6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>v</v>
+        <v>s</v>
       </c>
       <c r="Q6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="R6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>d</v>
+        <v>l</v>
       </c>
       <c r="S6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>l</v>
+        <v>m</v>
       </c>
       <c r="T6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -2327,27 +2330,27 @@
       </c>
       <c r="U6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>m</v>
+        <v>j</v>
       </c>
       <c r="V6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>j</v>
+        <v>v</v>
       </c>
       <c r="W6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>v</v>
+        <v>s</v>
       </c>
       <c r="X6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="Y6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>d</v>
+        <v>l</v>
       </c>
       <c r="Z6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>l</v>
+        <v>m</v>
       </c>
       <c r="AA6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -2355,27 +2358,27 @@
       </c>
       <c r="AB6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>m</v>
+        <v>j</v>
       </c>
       <c r="AC6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>j</v>
+        <v>v</v>
       </c>
       <c r="AD6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>v</v>
+        <v>s</v>
       </c>
       <c r="AE6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="AF6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>d</v>
+        <v>l</v>
       </c>
       <c r="AG6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>l</v>
+        <v>m</v>
       </c>
       <c r="AH6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -2383,27 +2386,27 @@
       </c>
       <c r="AI6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>m</v>
+        <v>j</v>
       </c>
       <c r="AJ6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>j</v>
+        <v>v</v>
       </c>
       <c r="AK6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>v</v>
+        <v>s</v>
       </c>
       <c r="AL6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="AM6" s="36" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>d</v>
+        <v>l</v>
       </c>
       <c r="AN6" s="36" t="str">
         <f t="shared" ref="AN6:BK6" ca="1" si="3">LEFT(TEXT(AN5,"jjj"),1)</f>
-        <v>l</v>
+        <v>m</v>
       </c>
       <c r="AO6" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2411,27 +2414,27 @@
       </c>
       <c r="AP6" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>j</v>
       </c>
       <c r="AQ6" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>v</v>
       </c>
       <c r="AR6" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>s</v>
       </c>
       <c r="AS6" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="AT6" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>l</v>
       </c>
       <c r="AU6" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>m</v>
       </c>
       <c r="AV6" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2439,27 +2442,27 @@
       </c>
       <c r="AW6" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>j</v>
       </c>
       <c r="AX6" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>v</v>
       </c>
       <c r="AY6" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>s</v>
       </c>
       <c r="AZ6" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="BA6" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>l</v>
       </c>
       <c r="BB6" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>m</v>
       </c>
       <c r="BC6" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2467,27 +2470,27 @@
       </c>
       <c r="BD6" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>j</v>
       </c>
       <c r="BE6" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>j</v>
+        <v>v</v>
       </c>
       <c r="BF6" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>v</v>
+        <v>s</v>
       </c>
       <c r="BG6" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>s</v>
+        <v>d</v>
       </c>
       <c r="BH6" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>d</v>
+        <v>l</v>
       </c>
       <c r="BI6" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>l</v>
+        <v>m</v>
       </c>
       <c r="BJ6" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2495,7 +2498,7 @@
       </c>
       <c r="BK6" s="36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>m</v>
+        <v>j</v>
       </c>
     </row>
     <row r="7" spans="1:63" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2569,7 +2572,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="62" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C8" s="22"/>
       <c r="D8" s="19"/>
@@ -2807,7 +2810,7 @@
         <v>22</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D9" s="19">
         <v>0</v>
@@ -2817,7 +2820,8 @@
         <v>43504</v>
       </c>
       <c r="F9" s="40">
-        <v>9</v>
+        <f>23</f>
+        <v>23</v>
       </c>
       <c r="G9" s="15"/>
       <c r="H9" s="61" t="str">
@@ -3048,20 +3052,20 @@
     <row r="10" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="24" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D10" s="19">
         <v>0</v>
       </c>
       <c r="E10" s="20">
-        <f>Début_Projet+55-35</f>
+        <f>Début_Projet+20</f>
         <v>43524</v>
       </c>
       <c r="F10" s="40">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="23" t="str">
@@ -3295,17 +3299,18 @@
         <v>23</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D11" s="19">
         <v>0</v>
       </c>
       <c r="E11" s="20">
-        <f>Début_Projet+20+7</f>
-        <v>43531</v>
+        <f>Début_Projet+23+25</f>
+        <v>43552</v>
       </c>
       <c r="F11" s="40">
-        <v>17</v>
+        <f>31</f>
+        <v>31</v>
       </c>
       <c r="G11" s="15"/>
       <c r="H11" s="23" t="str">
@@ -3534,266 +3539,258 @@
       </c>
     </row>
     <row r="12" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="19">
-        <v>0</v>
-      </c>
-      <c r="E12" s="20">
-        <f>Début_Projet+34+8</f>
-        <v>43546</v>
-      </c>
-      <c r="F12" s="40">
-        <v>16</v>
-      </c>
+      <c r="A12" s="10"/>
+      <c r="B12" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="22"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="40"/>
       <c r="G12" s="15"/>
       <c r="H12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(H$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(H$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="I12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(I$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(I$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="J12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(J$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(J$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="K12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(K$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(K$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="L12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(L$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(L$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="M12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(M$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(M$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="N12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(N$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(N$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="O12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(O$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(O$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="P12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(P$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(P$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="Q12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Q$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Q$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="R12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(R$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(R$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="S12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(S$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(S$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="T12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(T$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(T$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="U12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(U$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(U$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="V12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(V$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(V$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="W12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(W$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(W$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="X12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(X$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(X$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="Y12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Y$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Y$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="Z12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Z$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Z$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AA12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AA$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AA$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AB12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AB$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AB$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AC12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AC$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AC$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AD12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AD$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AD$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AE12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AE$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AE$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AF12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AF$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AF$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AG12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AG$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AG$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AH12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AH$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AH$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AI12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AI$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AI$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AJ12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AJ$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AJ$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AK12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AK$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AK$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AL12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AL$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AL$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AM12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AM$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AM$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AN12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AN$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AN$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AO12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AO$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AO$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AP12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AP$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AP$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AQ12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AQ$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AQ$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AR12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AR$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AR$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AS12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AS$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AS$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AT12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AT$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AT$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AU12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AU$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AU$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AV12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AV$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AV$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AW12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AW$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AW$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AX12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AX$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AX$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AY12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AY$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AY$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AZ12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AZ$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AZ$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BA12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BA$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BA$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BB12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BB$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BB$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BC12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BC$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BC$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BD12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BD$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BD$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BE12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BE$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BE$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BF12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BF$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BF$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BG12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BG$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BG$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BH12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BH$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BH$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BI12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BI$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BI$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BJ12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BJ$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BJ$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BK12" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BK$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BK$5=$E12,$F12=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
+      <c r="A13" s="10"/>
       <c r="B13" s="24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D13" s="19">
         <v>0</v>
       </c>
       <c r="E13" s="20">
-        <f>Début_Projet+48+8</f>
-        <v>43560</v>
+        <f>Début_Projet</f>
+        <v>43504</v>
       </c>
       <c r="F13" s="40">
-        <v>16</v>
+        <f>23</f>
+        <v>23</v>
       </c>
       <c r="G13" s="15"/>
       <c r="H13" s="23" t="str">
@@ -4022,257 +4019,266 @@
       </c>
     </row>
     <row r="14" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="62" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="40"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="19">
+        <v>0</v>
+      </c>
+      <c r="E14" s="20">
+        <f>Début_Projet+13+7</f>
+        <v>43524</v>
+      </c>
+      <c r="F14" s="40">
+        <v>38</v>
+      </c>
       <c r="G14" s="15"/>
       <c r="H14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(H$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(H$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="I14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(I$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(I$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="J14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(J$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(J$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="K14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(K$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(K$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="L14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(L$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(L$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="M14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(M$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(M$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="N14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(N$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(N$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="O14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(O$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(O$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="P14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(P$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(P$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="Q14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Q$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Q$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="R14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(R$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(R$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="S14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(S$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(S$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="T14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(T$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(T$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="U14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(U$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(U$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="V14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(V$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(V$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="W14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(W$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(W$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="X14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(X$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(X$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="Y14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Y$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Y$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="Z14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Z$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Z$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AA14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AA$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AA$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AB14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AB$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AB$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AC14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AC$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AC$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AD14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AD$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AD$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AE14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AE$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AE$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AF14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AF$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AF$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AG14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AG$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AG$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AH14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AH$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AH$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AI14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AI$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AI$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AJ14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AJ$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AJ$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AK14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AK$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AK$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AL14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AL$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AL$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AM14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AM$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AM$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AN14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AN$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AN$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AO14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AO$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AO$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AP14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AP$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AP$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AQ14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AQ$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AQ$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AR14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AR$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AR$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AS14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AS$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AS$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AT14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AT$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AT$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AU14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AU$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AU$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AV14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AV$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AV$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AW14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AW$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AW$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AX14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AX$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AX$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AY14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AY$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AY$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AZ14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AZ$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AZ$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BA14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BA$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BA$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BB14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BB$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BB$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BC14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BC$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BC$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BD14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BD$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BD$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BE14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BE$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BE$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BF14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BF$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BF$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BG14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BG$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BG$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BH14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BH$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BH$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BI14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BI$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BI$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BJ14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BJ$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BJ$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BK14" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BK$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BK$5=$E14,$F14=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
     </row>
     <row r="15" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D15" s="19">
         <v>0</v>
       </c>
       <c r="E15" s="20">
-        <f>Début_Projet</f>
-        <v>43504</v>
+        <f>Début_Projet+55</f>
+        <v>43559</v>
       </c>
       <c r="F15" s="40">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="23" t="str">
@@ -4503,20 +4509,20 @@
     <row r="16" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D16" s="19">
         <v>0</v>
       </c>
       <c r="E16" s="20">
-        <f>Début_Projet+13+7</f>
-        <v>43524</v>
+        <f>Début_Projet+69</f>
+        <v>43573</v>
       </c>
       <c r="F16" s="40">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G16" s="15"/>
       <c r="H16" s="23" t="str">
@@ -4746,265 +4752,256 @@
     </row>
     <row r="17" spans="1:66" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
-      <c r="B17" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="19">
-        <v>0</v>
-      </c>
-      <c r="E17" s="20">
-        <f>Début_Projet+34</f>
-        <v>43538</v>
-      </c>
-      <c r="F17" s="40">
-        <v>9</v>
-      </c>
+      <c r="B17" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="22"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="40"/>
       <c r="G17" s="15"/>
       <c r="H17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(H$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(H$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="I17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(I$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(I$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="J17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(J$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(J$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="K17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(K$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(K$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="L17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(L$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(L$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="M17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(M$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(M$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="N17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(N$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(N$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="O17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(O$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(O$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="P17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(P$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(P$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="Q17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Q$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Q$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="R17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(R$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(R$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="S17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(S$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(S$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="T17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(T$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(T$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="U17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(U$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(U$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="V17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(V$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(V$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="W17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(W$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(W$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="X17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(X$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(X$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="Y17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Y$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Y$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="Z17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Z$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Z$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AA17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AA$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AA$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AB17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AB$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AB$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AC17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AC$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AC$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AD17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AD$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AD$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AE17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AE$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AE$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AF17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AF$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AF$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AG17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AG$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AG$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AH17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AH$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AH$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AI17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AI$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AI$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AJ17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AJ$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AJ$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AK17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AK$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AK$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AL17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AL$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AL$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AM17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AM$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AM$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AN17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AN$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AN$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AO17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AO$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AO$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AP17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AP$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AP$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AQ17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AQ$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AQ$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AR17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AR$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AR$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AS17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AS$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AS$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AT17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AT$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AT$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AU17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AU$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AU$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AV17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AV$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AV$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AW17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AW$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AW$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AX17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AX$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AX$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AY17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AY$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AY$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="AZ17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AZ$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AZ$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BA17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BA$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BA$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BB17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BB$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BB$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BC17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BC$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BC$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BD17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BD$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BD$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BE17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BE$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BE$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BF17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BF$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BF$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BG17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BG$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BG$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BH17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BH$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BH$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BI17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BI$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BI$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BJ17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BJ$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BJ$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
       <c r="BK17" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BK$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
+        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BK$5=$E17,$F17=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:66" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D18" s="19">
         <v>0</v>
       </c>
       <c r="E18" s="20">
-        <f>Début_Projet+41</f>
-        <v>43545</v>
+        <f>Début_Projet</f>
+        <v>43504</v>
       </c>
       <c r="F18" s="40">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="G18" s="15"/>
       <c r="H18" s="23" t="str">
@@ -5235,20 +5232,20 @@
     <row r="19" spans="1:66" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D19" s="19">
         <v>0</v>
       </c>
       <c r="E19" s="20">
-        <f>Début_Projet+48</f>
-        <v>43552</v>
+        <f>Début_Projet+27</f>
+        <v>43531</v>
       </c>
       <c r="F19" s="40">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="G19" s="15"/>
       <c r="H19" s="23" t="str">
@@ -5478,487 +5475,319 @@
     </row>
     <row r="20" spans="1:66" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
-      <c r="B20" s="62" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="40"/>
+      <c r="B20" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="19">
+        <v>0</v>
+      </c>
+      <c r="E20" s="20">
+        <f>Début_Projet+48</f>
+        <v>43552</v>
+      </c>
+      <c r="F20" s="40">
+        <v>31</v>
+      </c>
       <c r="G20" s="15"/>
-      <c r="H20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(H$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="I20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(I$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="J20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(J$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="K20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(K$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="L20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(L$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="M20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(M$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="N20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(N$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="O20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(O$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="P20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(P$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="Q20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Q$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="R20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(R$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="S20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(S$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="T20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(T$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="U20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(U$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="V20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(V$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="W20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(W$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="X20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(X$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="Y20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Y$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="Z20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Z$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AA20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AA$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AB20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AB$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AC20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AC$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AD20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AD$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AE20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AE$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AF20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AF$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AG20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AG$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AH20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AH$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AI20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AI$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AJ20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AJ$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AK20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AK$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AL20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AL$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AM20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AM$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AN20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AN$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AO20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AO$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AP20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AP$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AQ20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AQ$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AR20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AR$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AS20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AS$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AT20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AT$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AU20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AU$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AV20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AV$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AW20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AW$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AX20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AX$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AY20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AY$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AZ20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AZ$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BA20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BA$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BB20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BB$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BC20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BC$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BD20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BD$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BE20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BE$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BF20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BF$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BG20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BG$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BH20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BH$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BI20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BI$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BJ20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BJ$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BK20" s="23" t="str">
-        <f>IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BK$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+      <c r="H20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(H$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="I20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(I$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="J20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(J$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="K20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(K$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="L20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(L$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="M20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(M$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="N20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(N$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="O20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(O$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="P20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(P$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="Q20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Q$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="R20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(R$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="S20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(S$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="T20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(T$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="U20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(U$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="V20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(V$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="W20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(W$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="X20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(X$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="Y20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Y$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="Z20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Z$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AA20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AA$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AB20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AB$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AC20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AC$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AD20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AD$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AE20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AE$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AF20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AF$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AG20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AG$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AH20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AH$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AI20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AI$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AJ20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AJ$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AK20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AK$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AL20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AL$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AM20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AM$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AN20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AN$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AO20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AO$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AP20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AP$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AQ20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AQ$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AR20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AR$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AS20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AS$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AT20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AT$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AU20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AU$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AV20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AV$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AW20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AW$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AX20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AX$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AY20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AY$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="AZ20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AZ$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BA20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BA$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BB20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BB$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BC20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BC$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BD20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BD$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BE20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BE$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BF20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BF$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BG20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BG$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BH20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BH$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BI20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BI$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BJ20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BJ$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
+        <v/>
+      </c>
+      <c r="BK20" s="45" t="str">
+        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BK$5=$E20,$F20=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
     </row>
     <row r="21" spans="1:66" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
-      <c r="B21" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="19">
-        <v>0</v>
-      </c>
-      <c r="E21" s="20">
-        <f>Début_Projet</f>
-        <v>43504</v>
-      </c>
-      <c r="F21" s="40">
-        <v>29</v>
-      </c>
+      <c r="A21" s="10"/>
+      <c r="B21" s="62" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="22"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="40"/>
       <c r="G21" s="15"/>
-      <c r="H21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(H$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="I21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(I$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="J21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(J$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="K21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(K$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="L21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(L$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="M21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(M$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="N21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(N$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="O21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(O$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="P21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(P$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="Q21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Q$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="R21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(R$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="S21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(S$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="T21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(T$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="U21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(U$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="V21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(V$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="W21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(W$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="X21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(X$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="Y21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Y$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="Z21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Z$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AA21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AA$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AB21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AB$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AC21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AC$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AD21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AD$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AE21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AE$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AF21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AF$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AG21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AG$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AH21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AH$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AI21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AI$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AJ21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AJ$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AK21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AK$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AL21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AL$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AM21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AM$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AN21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AN$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AO21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AO$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AP21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AP$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AQ21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AQ$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AR21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AR$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AS21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AS$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AT21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AT$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AU21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AU$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AV21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AV$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AW21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AW$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AX21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AX$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AY21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AY$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="AZ21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AZ$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BA21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BA$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BB21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BB$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BC21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BC$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BD21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BD$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BE21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BE$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BF21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BF$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BG21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BG$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BH21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BH$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BI21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BI$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BJ21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BJ$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
-      <c r="BK21" s="23" t="str">
-        <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BK$5=$E21,$F21=1),Marqueur_Jalon,"")),"")</f>
-        <v/>
-      </c>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="23"/>
+      <c r="P21" s="23"/>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="23"/>
+      <c r="S21" s="23"/>
+      <c r="T21" s="23"/>
+      <c r="U21" s="23"/>
+      <c r="V21" s="23"/>
+      <c r="W21" s="23"/>
+      <c r="X21" s="23"/>
+      <c r="Y21" s="23"/>
+      <c r="Z21" s="23"/>
+      <c r="AA21" s="23"/>
+      <c r="AB21" s="23"/>
+      <c r="AC21" s="23"/>
+      <c r="AD21" s="23"/>
+      <c r="AE21" s="23"/>
+      <c r="AF21" s="23"/>
+      <c r="AG21" s="23"/>
+      <c r="AH21" s="23"/>
+      <c r="AI21" s="23"/>
+      <c r="AJ21" s="23"/>
+      <c r="AK21" s="23"/>
+      <c r="AL21" s="23"/>
+      <c r="AM21" s="23"/>
+      <c r="AN21" s="23"/>
+      <c r="AO21" s="23"/>
+      <c r="AP21" s="23"/>
+      <c r="AQ21" s="23"/>
+      <c r="AR21" s="23"/>
+      <c r="AS21" s="23"/>
+      <c r="AT21" s="23"/>
+      <c r="AU21" s="23"/>
+      <c r="AV21" s="23"/>
+      <c r="AW21" s="23"/>
+      <c r="AX21" s="23"/>
+      <c r="AY21" s="23"/>
+      <c r="AZ21" s="23"/>
+      <c r="BA21" s="23"/>
+      <c r="BB21" s="23"/>
+      <c r="BC21" s="23"/>
+      <c r="BD21" s="23"/>
+      <c r="BE21" s="23"/>
+      <c r="BF21" s="23"/>
+      <c r="BG21" s="23"/>
+      <c r="BH21" s="23"/>
+      <c r="BI21" s="23"/>
+      <c r="BJ21" s="23"/>
+      <c r="BK21" s="23"/>
     </row>
     <row r="22" spans="1:66" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="24" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C22" s="22" t="s">
         <v>40</v>
@@ -5967,11 +5796,11 @@
         <v>0</v>
       </c>
       <c r="E22" s="20">
-        <f>Début_Projet+27</f>
-        <v>43531</v>
+        <f>Début_Projet+76</f>
+        <v>43580</v>
       </c>
       <c r="F22" s="40">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G22" s="15"/>
       <c r="H22" s="23" t="str">
@@ -6202,7 +6031,7 @@
     <row r="23" spans="1:66" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="24" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C23" s="22" t="s">
         <v>40</v>
@@ -6211,313 +6040,453 @@
         <v>0</v>
       </c>
       <c r="E23" s="20">
-        <f>Début_Projet+34</f>
-        <v>43538</v>
+        <f>Début_Projet+76</f>
+        <v>43580</v>
       </c>
       <c r="F23" s="40">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="G23" s="15"/>
-      <c r="H23" s="45" t="str">
+      <c r="H23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(H$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="I23" s="45" t="str">
+      <c r="I23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(I$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="J23" s="45" t="str">
+      <c r="J23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(J$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="K23" s="45" t="str">
+      <c r="K23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(K$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="L23" s="45" t="str">
+      <c r="L23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(L$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="M23" s="45" t="str">
+      <c r="M23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(M$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="N23" s="45" t="str">
+      <c r="N23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(N$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="O23" s="45" t="str">
+      <c r="O23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(O$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="P23" s="45" t="str">
+      <c r="P23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(P$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="Q23" s="45" t="str">
+      <c r="Q23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Q$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="R23" s="45" t="str">
+      <c r="R23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(R$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="S23" s="45" t="str">
+      <c r="S23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(S$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="T23" s="45" t="str">
+      <c r="T23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(T$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="U23" s="45" t="str">
+      <c r="U23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(U$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="V23" s="45" t="str">
+      <c r="V23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(V$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="W23" s="45" t="str">
+      <c r="W23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(W$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="X23" s="45" t="str">
+      <c r="X23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(X$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="Y23" s="45" t="str">
+      <c r="Y23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Y$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="Z23" s="45" t="str">
+      <c r="Z23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(Z$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="AA23" s="45" t="str">
+      <c r="AA23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AA$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="AB23" s="45" t="str">
+      <c r="AB23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AB$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="AC23" s="45" t="str">
+      <c r="AC23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AC$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="AD23" s="45" t="str">
+      <c r="AD23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AD$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="AE23" s="45" t="str">
+      <c r="AE23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AE$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="AF23" s="45" t="str">
+      <c r="AF23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AF$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="AG23" s="45" t="str">
+      <c r="AG23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AG$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="AH23" s="45" t="str">
+      <c r="AH23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AH$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="AI23" s="45" t="str">
+      <c r="AI23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AI$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="AJ23" s="45" t="str">
+      <c r="AJ23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AJ$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="AK23" s="45" t="str">
+      <c r="AK23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AK$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="AL23" s="45" t="str">
+      <c r="AL23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AL$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="AM23" s="45" t="str">
+      <c r="AM23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AM$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="AN23" s="45" t="str">
+      <c r="AN23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AN$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="AO23" s="45" t="str">
+      <c r="AO23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AO$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="AP23" s="45" t="str">
+      <c r="AP23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AP$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="AQ23" s="45" t="str">
+      <c r="AQ23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AQ$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="AR23" s="45" t="str">
+      <c r="AR23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AR$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="AS23" s="45" t="str">
+      <c r="AS23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AS$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="AT23" s="45" t="str">
+      <c r="AT23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AT$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="AU23" s="45" t="str">
+      <c r="AU23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AU$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="AV23" s="45" t="str">
+      <c r="AV23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AV$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="AW23" s="45" t="str">
+      <c r="AW23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AW$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="AX23" s="45" t="str">
+      <c r="AX23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AX$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="AY23" s="45" t="str">
+      <c r="AY23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AY$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="AZ23" s="45" t="str">
+      <c r="AZ23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(AZ$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="BA23" s="45" t="str">
+      <c r="BA23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BA$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="BB23" s="45" t="str">
+      <c r="BB23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BB$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="BC23" s="45" t="str">
+      <c r="BC23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BC$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="BD23" s="45" t="str">
+      <c r="BD23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BD$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="BE23" s="45" t="str">
+      <c r="BE23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BE$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="BF23" s="45" t="str">
+      <c r="BF23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BF$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="BG23" s="45" t="str">
+      <c r="BG23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BG$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="BH23" s="45" t="str">
+      <c r="BH23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BH$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="BI23" s="45" t="str">
+      <c r="BI23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BI$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="BJ23" s="45" t="str">
+      <c r="BJ23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BJ$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
-      <c r="BK23" s="45" t="str">
+      <c r="BK23" s="23" t="str">
         <f ca="1">IFERROR(IF(LEN(Jalons[[#This Row],[Nombre de jours]])=0,"",IF(AND(BK$5=$E23,$F23=1),Marqueur_Jalon,"")),"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:66" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="46"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="50"/>
-      <c r="G24" s="51"/>
-      <c r="H24" s="52"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="52"/>
-      <c r="K24" s="52"/>
-      <c r="L24" s="52"/>
-      <c r="M24" s="52"/>
-      <c r="N24" s="52"/>
-      <c r="O24" s="52"/>
-      <c r="P24" s="52"/>
-      <c r="Q24" s="52"/>
-      <c r="R24" s="52"/>
-      <c r="S24" s="52"/>
-      <c r="T24" s="52"/>
-      <c r="U24" s="52"/>
-      <c r="V24" s="52"/>
-      <c r="W24" s="52"/>
-      <c r="X24" s="52"/>
-      <c r="Y24" s="52"/>
-      <c r="Z24" s="52"/>
-      <c r="AA24" s="52"/>
-      <c r="AB24" s="52"/>
-      <c r="AC24" s="52"/>
-      <c r="AD24" s="52"/>
-      <c r="AE24" s="52"/>
-      <c r="AF24" s="52"/>
-      <c r="AG24" s="52"/>
-      <c r="AH24" s="52"/>
-      <c r="AI24" s="52"/>
-      <c r="AJ24" s="52"/>
-      <c r="AK24" s="52"/>
-      <c r="AL24" s="52"/>
-      <c r="AM24" s="52"/>
-      <c r="AN24" s="52"/>
-      <c r="AO24" s="52"/>
-      <c r="AP24" s="52"/>
-      <c r="AQ24" s="52"/>
-      <c r="AR24" s="52"/>
-      <c r="AS24" s="52"/>
-      <c r="AT24" s="52"/>
-      <c r="AU24" s="52"/>
-      <c r="AV24" s="52"/>
-      <c r="AW24" s="52"/>
-      <c r="AX24" s="52"/>
-      <c r="AY24" s="52"/>
-      <c r="AZ24" s="52"/>
-      <c r="BA24" s="52"/>
-      <c r="BB24" s="52"/>
-      <c r="BC24" s="52"/>
-      <c r="BD24" s="52"/>
-      <c r="BE24" s="52"/>
-      <c r="BF24" s="52"/>
-      <c r="BG24" s="52"/>
-      <c r="BH24" s="52"/>
-      <c r="BI24" s="52"/>
-      <c r="BJ24" s="52"/>
-      <c r="BK24" s="52"/>
-      <c r="BL24" s="53"/>
-      <c r="BM24" s="53"/>
-      <c r="BN24" s="53"/>
+    <row r="27" spans="1:66" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="9"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="52"/>
+      <c r="L27" s="52"/>
+      <c r="M27" s="52"/>
+      <c r="N27" s="52"/>
+      <c r="O27" s="52"/>
+      <c r="P27" s="52"/>
+      <c r="Q27" s="52"/>
+      <c r="R27" s="52"/>
+      <c r="S27" s="52"/>
+      <c r="T27" s="52"/>
+      <c r="U27" s="52"/>
+      <c r="V27" s="52"/>
+      <c r="W27" s="52"/>
+      <c r="X27" s="52"/>
+      <c r="Y27" s="52"/>
+      <c r="Z27" s="52"/>
+      <c r="AA27" s="52"/>
+      <c r="AB27" s="52"/>
+      <c r="AC27" s="52"/>
+      <c r="AD27" s="52"/>
+      <c r="AE27" s="52"/>
+      <c r="AF27" s="52"/>
+      <c r="AG27" s="52"/>
+      <c r="AH27" s="52"/>
+      <c r="AI27" s="52"/>
+      <c r="AJ27" s="52"/>
+      <c r="AK27" s="52"/>
+      <c r="AL27" s="52"/>
+      <c r="AM27" s="52"/>
+      <c r="AN27" s="52"/>
+      <c r="AO27" s="52"/>
+      <c r="AP27" s="52"/>
+      <c r="AQ27" s="52"/>
+      <c r="AR27" s="52"/>
+      <c r="AS27" s="52"/>
+      <c r="AT27" s="52"/>
+      <c r="AU27" s="52"/>
+      <c r="AV27" s="52"/>
+      <c r="AW27" s="52"/>
+      <c r="AX27" s="52"/>
+      <c r="AY27" s="52"/>
+      <c r="AZ27" s="52"/>
+      <c r="BA27" s="52"/>
+      <c r="BB27" s="52"/>
+      <c r="BC27" s="52"/>
+      <c r="BD27" s="52"/>
+      <c r="BE27" s="52"/>
+      <c r="BF27" s="52"/>
+      <c r="BG27" s="52"/>
+      <c r="BH27" s="52"/>
+      <c r="BI27" s="52"/>
+      <c r="BJ27" s="52"/>
+      <c r="BK27" s="52"/>
+      <c r="BL27" s="53"/>
+      <c r="BM27" s="53"/>
+      <c r="BN27" s="53"/>
+    </row>
+    <row r="28" spans="1:66" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
+      <c r="B28" s="46"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="52"/>
+      <c r="J28" s="52"/>
+      <c r="K28" s="52"/>
+      <c r="L28" s="52"/>
+      <c r="M28" s="52"/>
+      <c r="N28" s="52"/>
+      <c r="O28" s="52"/>
+      <c r="P28" s="52"/>
+      <c r="Q28" s="52"/>
+      <c r="R28" s="52"/>
+      <c r="S28" s="52"/>
+      <c r="T28" s="52"/>
+      <c r="U28" s="52"/>
+      <c r="V28" s="52"/>
+      <c r="W28" s="52"/>
+      <c r="X28" s="52"/>
+      <c r="Y28" s="52"/>
+      <c r="Z28" s="52"/>
+      <c r="AA28" s="52"/>
+      <c r="AB28" s="52"/>
+      <c r="AC28" s="52"/>
+      <c r="AD28" s="52"/>
+      <c r="AE28" s="52"/>
+      <c r="AF28" s="52"/>
+      <c r="AG28" s="52"/>
+      <c r="AH28" s="52"/>
+      <c r="AI28" s="52"/>
+      <c r="AJ28" s="52"/>
+      <c r="AK28" s="52"/>
+      <c r="AL28" s="52"/>
+      <c r="AM28" s="52"/>
+      <c r="AN28" s="52"/>
+      <c r="AO28" s="52"/>
+      <c r="AP28" s="52"/>
+      <c r="AQ28" s="52"/>
+      <c r="AR28" s="52"/>
+      <c r="AS28" s="52"/>
+      <c r="AT28" s="52"/>
+      <c r="AU28" s="52"/>
+      <c r="AV28" s="52"/>
+      <c r="AW28" s="52"/>
+      <c r="AX28" s="52"/>
+      <c r="AY28" s="52"/>
+      <c r="AZ28" s="52"/>
+      <c r="BA28" s="52"/>
+      <c r="BB28" s="52"/>
+      <c r="BC28" s="52"/>
+      <c r="BD28" s="52"/>
+      <c r="BE28" s="52"/>
+      <c r="BF28" s="52"/>
+      <c r="BG28" s="52"/>
+      <c r="BH28" s="52"/>
+      <c r="BI28" s="52"/>
+      <c r="BJ28" s="52"/>
+      <c r="BK28" s="52"/>
+      <c r="BL28" s="53"/>
+      <c r="BM28" s="53"/>
+      <c r="BN28" s="53"/>
+    </row>
+    <row r="29" spans="1:66" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="46"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="52"/>
+      <c r="L29" s="52"/>
+      <c r="M29" s="52"/>
+      <c r="N29" s="52"/>
+      <c r="O29" s="52"/>
+      <c r="P29" s="52"/>
+      <c r="Q29" s="52"/>
+      <c r="R29" s="52"/>
+      <c r="S29" s="52"/>
+      <c r="T29" s="52"/>
+      <c r="U29" s="52"/>
+      <c r="V29" s="52"/>
+      <c r="W29" s="52"/>
+      <c r="X29" s="52"/>
+      <c r="Y29" s="52"/>
+      <c r="Z29" s="52"/>
+      <c r="AA29" s="52"/>
+      <c r="AB29" s="52"/>
+      <c r="AC29" s="52"/>
+      <c r="AD29" s="52"/>
+      <c r="AE29" s="52"/>
+      <c r="AF29" s="52"/>
+      <c r="AG29" s="52"/>
+      <c r="AH29" s="52"/>
+      <c r="AI29" s="52"/>
+      <c r="AJ29" s="52"/>
+      <c r="AK29" s="52"/>
+      <c r="AL29" s="52"/>
+      <c r="AM29" s="52"/>
+      <c r="AN29" s="52"/>
+      <c r="AO29" s="52"/>
+      <c r="AP29" s="52"/>
+      <c r="AQ29" s="52"/>
+      <c r="AR29" s="52"/>
+      <c r="AS29" s="52"/>
+      <c r="AT29" s="52"/>
+      <c r="AU29" s="52"/>
+      <c r="AV29" s="52"/>
+      <c r="AW29" s="52"/>
+      <c r="AX29" s="52"/>
+      <c r="AY29" s="52"/>
+      <c r="AZ29" s="52"/>
+      <c r="BA29" s="52"/>
+      <c r="BB29" s="52"/>
+      <c r="BC29" s="52"/>
+      <c r="BD29" s="52"/>
+      <c r="BE29" s="52"/>
+      <c r="BF29" s="52"/>
+      <c r="BG29" s="52"/>
+      <c r="BH29" s="52"/>
+      <c r="BI29" s="52"/>
+      <c r="BJ29" s="52"/>
+      <c r="BK29" s="52"/>
+      <c r="BL29" s="53"/>
+      <c r="BM29" s="53"/>
+      <c r="BN29" s="53"/>
     </row>
     <row r="30" spans="1:66" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
-      <c r="B30" s="46"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="50"/>
+      <c r="A30" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="54"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="54"/>
       <c r="G30" s="51"/>
       <c r="H30" s="52"/>
       <c r="I30" s="52"/>
@@ -6579,221 +6548,214 @@
       <c r="BM30" s="53"/>
       <c r="BN30" s="53"/>
     </row>
-    <row r="31" spans="1:66" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
-      <c r="B31" s="46"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="51"/>
-      <c r="H31" s="52"/>
-      <c r="I31" s="52"/>
-      <c r="J31" s="52"/>
-      <c r="K31" s="52"/>
-      <c r="L31" s="52"/>
-      <c r="M31" s="52"/>
-      <c r="N31" s="52"/>
-      <c r="O31" s="52"/>
-      <c r="P31" s="52"/>
-      <c r="Q31" s="52"/>
-      <c r="R31" s="52"/>
-      <c r="S31" s="52"/>
-      <c r="T31" s="52"/>
-      <c r="U31" s="52"/>
-      <c r="V31" s="52"/>
-      <c r="W31" s="52"/>
-      <c r="X31" s="52"/>
-      <c r="Y31" s="52"/>
-      <c r="Z31" s="52"/>
-      <c r="AA31" s="52"/>
-      <c r="AB31" s="52"/>
-      <c r="AC31" s="52"/>
-      <c r="AD31" s="52"/>
-      <c r="AE31" s="52"/>
-      <c r="AF31" s="52"/>
-      <c r="AG31" s="52"/>
-      <c r="AH31" s="52"/>
-      <c r="AI31" s="52"/>
-      <c r="AJ31" s="52"/>
-      <c r="AK31" s="52"/>
-      <c r="AL31" s="52"/>
-      <c r="AM31" s="52"/>
-      <c r="AN31" s="52"/>
-      <c r="AO31" s="52"/>
-      <c r="AP31" s="52"/>
-      <c r="AQ31" s="52"/>
-      <c r="AR31" s="52"/>
-      <c r="AS31" s="52"/>
-      <c r="AT31" s="52"/>
-      <c r="AU31" s="52"/>
-      <c r="AV31" s="52"/>
-      <c r="AW31" s="52"/>
-      <c r="AX31" s="52"/>
-      <c r="AY31" s="52"/>
-      <c r="AZ31" s="52"/>
-      <c r="BA31" s="52"/>
-      <c r="BB31" s="52"/>
-      <c r="BC31" s="52"/>
-      <c r="BD31" s="52"/>
-      <c r="BE31" s="52"/>
-      <c r="BF31" s="52"/>
-      <c r="BG31" s="52"/>
-      <c r="BH31" s="52"/>
-      <c r="BI31" s="52"/>
-      <c r="BJ31" s="52"/>
-      <c r="BK31" s="52"/>
-      <c r="BL31" s="53"/>
-      <c r="BM31" s="53"/>
-      <c r="BN31" s="53"/>
+    <row r="31" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="54"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="54"/>
+      <c r="I31" s="54"/>
+      <c r="J31" s="54"/>
+      <c r="K31" s="54"/>
+      <c r="L31" s="54"/>
+      <c r="M31" s="54"/>
+      <c r="N31" s="54"/>
+      <c r="O31" s="54"/>
+      <c r="P31" s="54"/>
+      <c r="Q31" s="54"/>
+      <c r="R31" s="54"/>
+      <c r="S31" s="54"/>
+      <c r="T31" s="54"/>
+      <c r="U31" s="54"/>
+      <c r="V31" s="54"/>
+      <c r="W31" s="54"/>
+      <c r="X31" s="54"/>
+      <c r="Y31" s="54"/>
+      <c r="Z31" s="54"/>
+      <c r="AA31" s="54"/>
+      <c r="AB31" s="54"/>
+      <c r="AC31" s="54"/>
+      <c r="AD31" s="54"/>
+      <c r="AE31" s="54"/>
+      <c r="AF31" s="54"/>
+      <c r="AG31" s="54"/>
+      <c r="AH31" s="54"/>
+      <c r="AI31" s="54"/>
+      <c r="AJ31" s="54"/>
+      <c r="AK31" s="54"/>
+      <c r="AL31" s="54"/>
+      <c r="AM31" s="54"/>
+      <c r="AN31" s="54"/>
+      <c r="AO31" s="54"/>
+      <c r="AP31" s="54"/>
+      <c r="AQ31" s="54"/>
+      <c r="AR31" s="54"/>
+      <c r="AS31" s="54"/>
+      <c r="AT31" s="54"/>
+      <c r="AU31" s="54"/>
+      <c r="AV31" s="54"/>
+      <c r="AW31" s="54"/>
+      <c r="AX31" s="54"/>
+      <c r="AY31" s="54"/>
+      <c r="AZ31" s="54"/>
+      <c r="BA31" s="54"/>
+      <c r="BB31" s="54"/>
+      <c r="BC31" s="54"/>
+      <c r="BD31" s="54"/>
+      <c r="BE31" s="54"/>
+      <c r="BF31" s="54"/>
+      <c r="BG31" s="54"/>
+      <c r="BH31" s="54"/>
+      <c r="BI31" s="54"/>
+      <c r="BJ31" s="54"/>
+      <c r="BK31" s="54"/>
+      <c r="BL31" s="54"/>
+      <c r="BM31" s="54"/>
+      <c r="BN31" s="54"/>
     </row>
-    <row r="32" spans="1:66" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" s="46"/>
-      <c r="C32" s="47"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="49"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="51"/>
-      <c r="H32" s="52"/>
-      <c r="I32" s="52"/>
-      <c r="J32" s="52"/>
-      <c r="K32" s="52"/>
-      <c r="L32" s="52"/>
-      <c r="M32" s="52"/>
-      <c r="N32" s="52"/>
-      <c r="O32" s="52"/>
-      <c r="P32" s="52"/>
-      <c r="Q32" s="52"/>
-      <c r="R32" s="52"/>
-      <c r="S32" s="52"/>
-      <c r="T32" s="52"/>
-      <c r="U32" s="52"/>
-      <c r="V32" s="52"/>
-      <c r="W32" s="52"/>
-      <c r="X32" s="52"/>
-      <c r="Y32" s="52"/>
-      <c r="Z32" s="52"/>
-      <c r="AA32" s="52"/>
-      <c r="AB32" s="52"/>
-      <c r="AC32" s="52"/>
-      <c r="AD32" s="52"/>
-      <c r="AE32" s="52"/>
-      <c r="AF32" s="52"/>
-      <c r="AG32" s="52"/>
-      <c r="AH32" s="52"/>
-      <c r="AI32" s="52"/>
-      <c r="AJ32" s="52"/>
-      <c r="AK32" s="52"/>
-      <c r="AL32" s="52"/>
-      <c r="AM32" s="52"/>
-      <c r="AN32" s="52"/>
-      <c r="AO32" s="52"/>
-      <c r="AP32" s="52"/>
-      <c r="AQ32" s="52"/>
-      <c r="AR32" s="52"/>
-      <c r="AS32" s="52"/>
-      <c r="AT32" s="52"/>
-      <c r="AU32" s="52"/>
-      <c r="AV32" s="52"/>
-      <c r="AW32" s="52"/>
-      <c r="AX32" s="52"/>
-      <c r="AY32" s="52"/>
-      <c r="AZ32" s="52"/>
-      <c r="BA32" s="52"/>
-      <c r="BB32" s="52"/>
-      <c r="BC32" s="52"/>
-      <c r="BD32" s="52"/>
-      <c r="BE32" s="52"/>
-      <c r="BF32" s="52"/>
-      <c r="BG32" s="52"/>
-      <c r="BH32" s="52"/>
-      <c r="BI32" s="52"/>
-      <c r="BJ32" s="52"/>
-      <c r="BK32" s="52"/>
-      <c r="BL32" s="53"/>
-      <c r="BM32" s="53"/>
-      <c r="BN32" s="53"/>
+    <row r="32" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="54"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="54"/>
+      <c r="H32" s="54"/>
+      <c r="I32" s="54"/>
+      <c r="J32" s="54"/>
+      <c r="K32" s="54"/>
+      <c r="L32" s="54"/>
+      <c r="M32" s="54"/>
+      <c r="N32" s="54"/>
+      <c r="O32" s="54"/>
+      <c r="P32" s="54"/>
+      <c r="Q32" s="54"/>
+      <c r="R32" s="54"/>
+      <c r="S32" s="54"/>
+      <c r="T32" s="54"/>
+      <c r="U32" s="54"/>
+      <c r="V32" s="54"/>
+      <c r="W32" s="54"/>
+      <c r="X32" s="54"/>
+      <c r="Y32" s="54"/>
+      <c r="Z32" s="54"/>
+      <c r="AA32" s="54"/>
+      <c r="AB32" s="54"/>
+      <c r="AC32" s="54"/>
+      <c r="AD32" s="54"/>
+      <c r="AE32" s="54"/>
+      <c r="AF32" s="54"/>
+      <c r="AG32" s="54"/>
+      <c r="AH32" s="54"/>
+      <c r="AI32" s="54"/>
+      <c r="AJ32" s="54"/>
+      <c r="AK32" s="54"/>
+      <c r="AL32" s="54"/>
+      <c r="AM32" s="54"/>
+      <c r="AN32" s="54"/>
+      <c r="AO32" s="54"/>
+      <c r="AP32" s="54"/>
+      <c r="AQ32" s="54"/>
+      <c r="AR32" s="54"/>
+      <c r="AS32" s="54"/>
+      <c r="AT32" s="54"/>
+      <c r="AU32" s="54"/>
+      <c r="AV32" s="54"/>
+      <c r="AW32" s="54"/>
+      <c r="AX32" s="54"/>
+      <c r="AY32" s="54"/>
+      <c r="AZ32" s="54"/>
+      <c r="BA32" s="54"/>
+      <c r="BB32" s="54"/>
+      <c r="BC32" s="54"/>
+      <c r="BD32" s="54"/>
+      <c r="BE32" s="54"/>
+      <c r="BF32" s="54"/>
+      <c r="BG32" s="54"/>
+      <c r="BH32" s="54"/>
+      <c r="BI32" s="54"/>
+      <c r="BJ32" s="54"/>
+      <c r="BK32" s="54"/>
+      <c r="BL32" s="54"/>
+      <c r="BM32" s="54"/>
+      <c r="BN32" s="54"/>
     </row>
-    <row r="33" spans="1:66" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
-        <v>9</v>
-      </c>
+    <row r="33" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="54"/>
       <c r="C33" s="54"/>
       <c r="D33" s="54"/>
       <c r="E33" s="55"/>
       <c r="F33" s="54"/>
-      <c r="G33" s="51"/>
-      <c r="H33" s="52"/>
-      <c r="I33" s="52"/>
-      <c r="J33" s="52"/>
-      <c r="K33" s="52"/>
-      <c r="L33" s="52"/>
-      <c r="M33" s="52"/>
-      <c r="N33" s="52"/>
-      <c r="O33" s="52"/>
-      <c r="P33" s="52"/>
-      <c r="Q33" s="52"/>
-      <c r="R33" s="52"/>
-      <c r="S33" s="52"/>
-      <c r="T33" s="52"/>
-      <c r="U33" s="52"/>
-      <c r="V33" s="52"/>
-      <c r="W33" s="52"/>
-      <c r="X33" s="52"/>
-      <c r="Y33" s="52"/>
-      <c r="Z33" s="52"/>
-      <c r="AA33" s="52"/>
-      <c r="AB33" s="52"/>
-      <c r="AC33" s="52"/>
-      <c r="AD33" s="52"/>
-      <c r="AE33" s="52"/>
-      <c r="AF33" s="52"/>
-      <c r="AG33" s="52"/>
-      <c r="AH33" s="52"/>
-      <c r="AI33" s="52"/>
-      <c r="AJ33" s="52"/>
-      <c r="AK33" s="52"/>
-      <c r="AL33" s="52"/>
-      <c r="AM33" s="52"/>
-      <c r="AN33" s="52"/>
-      <c r="AO33" s="52"/>
-      <c r="AP33" s="52"/>
-      <c r="AQ33" s="52"/>
-      <c r="AR33" s="52"/>
-      <c r="AS33" s="52"/>
-      <c r="AT33" s="52"/>
-      <c r="AU33" s="52"/>
-      <c r="AV33" s="52"/>
-      <c r="AW33" s="52"/>
-      <c r="AX33" s="52"/>
-      <c r="AY33" s="52"/>
-      <c r="AZ33" s="52"/>
-      <c r="BA33" s="52"/>
-      <c r="BB33" s="52"/>
-      <c r="BC33" s="52"/>
-      <c r="BD33" s="52"/>
-      <c r="BE33" s="52"/>
-      <c r="BF33" s="52"/>
-      <c r="BG33" s="52"/>
-      <c r="BH33" s="52"/>
-      <c r="BI33" s="52"/>
-      <c r="BJ33" s="52"/>
-      <c r="BK33" s="52"/>
-      <c r="BL33" s="53"/>
-      <c r="BM33" s="53"/>
-      <c r="BN33" s="53"/>
+      <c r="G33" s="54"/>
+      <c r="H33" s="54"/>
+      <c r="I33" s="54"/>
+      <c r="J33" s="54"/>
+      <c r="K33" s="54"/>
+      <c r="L33" s="54"/>
+      <c r="M33" s="54"/>
+      <c r="N33" s="54"/>
+      <c r="O33" s="54"/>
+      <c r="P33" s="54"/>
+      <c r="Q33" s="54"/>
+      <c r="R33" s="54"/>
+      <c r="S33" s="54"/>
+      <c r="T33" s="54"/>
+      <c r="U33" s="54"/>
+      <c r="V33" s="54"/>
+      <c r="W33" s="54"/>
+      <c r="X33" s="54"/>
+      <c r="Y33" s="54"/>
+      <c r="Z33" s="54"/>
+      <c r="AA33" s="54"/>
+      <c r="AB33" s="54"/>
+      <c r="AC33" s="54"/>
+      <c r="AD33" s="54"/>
+      <c r="AE33" s="54"/>
+      <c r="AF33" s="54"/>
+      <c r="AG33" s="54"/>
+      <c r="AH33" s="54"/>
+      <c r="AI33" s="54"/>
+      <c r="AJ33" s="54"/>
+      <c r="AK33" s="54"/>
+      <c r="AL33" s="54"/>
+      <c r="AM33" s="54"/>
+      <c r="AN33" s="54"/>
+      <c r="AO33" s="54"/>
+      <c r="AP33" s="54"/>
+      <c r="AQ33" s="54"/>
+      <c r="AR33" s="54"/>
+      <c r="AS33" s="54"/>
+      <c r="AT33" s="54"/>
+      <c r="AU33" s="54"/>
+      <c r="AV33" s="54"/>
+      <c r="AW33" s="54"/>
+      <c r="AX33" s="54"/>
+      <c r="AY33" s="54"/>
+      <c r="AZ33" s="54"/>
+      <c r="BA33" s="54"/>
+      <c r="BB33" s="54"/>
+      <c r="BC33" s="54"/>
+      <c r="BD33" s="54"/>
+      <c r="BE33" s="54"/>
+      <c r="BF33" s="54"/>
+      <c r="BG33" s="54"/>
+      <c r="BH33" s="54"/>
+      <c r="BI33" s="54"/>
+      <c r="BJ33" s="54"/>
+      <c r="BK33" s="54"/>
+      <c r="BL33" s="54"/>
+      <c r="BM33" s="54"/>
+      <c r="BN33" s="54"/>
     </row>
-    <row r="34" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="54"/>
-      <c r="C34" s="56"/>
+      <c r="C34" s="54"/>
       <c r="D34" s="54"/>
       <c r="E34" s="55"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="58"/>
+      <c r="F34" s="54"/>
+      <c r="G34" s="54"/>
       <c r="H34" s="54"/>
       <c r="I34" s="54"/>
       <c r="J34" s="54"/>
@@ -6854,9 +6816,9 @@
       <c r="BM34" s="54"/>
       <c r="BN34" s="54"/>
     </row>
-    <row r="35" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="54"/>
-      <c r="C35" s="59"/>
+      <c r="C35" s="54"/>
       <c r="D35" s="54"/>
       <c r="E35" s="55"/>
       <c r="F35" s="54"/>
@@ -6921,7 +6883,7 @@
       <c r="BM35" s="54"/>
       <c r="BN35" s="54"/>
     </row>
-    <row r="36" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="54"/>
       <c r="C36" s="54"/>
       <c r="D36" s="54"/>
@@ -6988,7 +6950,7 @@
       <c r="BM36" s="54"/>
       <c r="BN36" s="54"/>
     </row>
-    <row r="37" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="54"/>
       <c r="C37" s="54"/>
       <c r="D37" s="54"/>
@@ -7055,207 +7017,6 @@
       <c r="BM37" s="54"/>
       <c r="BN37" s="54"/>
     </row>
-    <row r="38" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="54"/>
-      <c r="C38" s="54"/>
-      <c r="D38" s="54"/>
-      <c r="E38" s="55"/>
-      <c r="F38" s="54"/>
-      <c r="G38" s="54"/>
-      <c r="H38" s="54"/>
-      <c r="I38" s="54"/>
-      <c r="J38" s="54"/>
-      <c r="K38" s="54"/>
-      <c r="L38" s="54"/>
-      <c r="M38" s="54"/>
-      <c r="N38" s="54"/>
-      <c r="O38" s="54"/>
-      <c r="P38" s="54"/>
-      <c r="Q38" s="54"/>
-      <c r="R38" s="54"/>
-      <c r="S38" s="54"/>
-      <c r="T38" s="54"/>
-      <c r="U38" s="54"/>
-      <c r="V38" s="54"/>
-      <c r="W38" s="54"/>
-      <c r="X38" s="54"/>
-      <c r="Y38" s="54"/>
-      <c r="Z38" s="54"/>
-      <c r="AA38" s="54"/>
-      <c r="AB38" s="54"/>
-      <c r="AC38" s="54"/>
-      <c r="AD38" s="54"/>
-      <c r="AE38" s="54"/>
-      <c r="AF38" s="54"/>
-      <c r="AG38" s="54"/>
-      <c r="AH38" s="54"/>
-      <c r="AI38" s="54"/>
-      <c r="AJ38" s="54"/>
-      <c r="AK38" s="54"/>
-      <c r="AL38" s="54"/>
-      <c r="AM38" s="54"/>
-      <c r="AN38" s="54"/>
-      <c r="AO38" s="54"/>
-      <c r="AP38" s="54"/>
-      <c r="AQ38" s="54"/>
-      <c r="AR38" s="54"/>
-      <c r="AS38" s="54"/>
-      <c r="AT38" s="54"/>
-      <c r="AU38" s="54"/>
-      <c r="AV38" s="54"/>
-      <c r="AW38" s="54"/>
-      <c r="AX38" s="54"/>
-      <c r="AY38" s="54"/>
-      <c r="AZ38" s="54"/>
-      <c r="BA38" s="54"/>
-      <c r="BB38" s="54"/>
-      <c r="BC38" s="54"/>
-      <c r="BD38" s="54"/>
-      <c r="BE38" s="54"/>
-      <c r="BF38" s="54"/>
-      <c r="BG38" s="54"/>
-      <c r="BH38" s="54"/>
-      <c r="BI38" s="54"/>
-      <c r="BJ38" s="54"/>
-      <c r="BK38" s="54"/>
-      <c r="BL38" s="54"/>
-      <c r="BM38" s="54"/>
-      <c r="BN38" s="54"/>
-    </row>
-    <row r="39" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="54"/>
-      <c r="C39" s="54"/>
-      <c r="D39" s="54"/>
-      <c r="E39" s="55"/>
-      <c r="F39" s="54"/>
-      <c r="G39" s="54"/>
-      <c r="H39" s="54"/>
-      <c r="I39" s="54"/>
-      <c r="J39" s="54"/>
-      <c r="K39" s="54"/>
-      <c r="L39" s="54"/>
-      <c r="M39" s="54"/>
-      <c r="N39" s="54"/>
-      <c r="O39" s="54"/>
-      <c r="P39" s="54"/>
-      <c r="Q39" s="54"/>
-      <c r="R39" s="54"/>
-      <c r="S39" s="54"/>
-      <c r="T39" s="54"/>
-      <c r="U39" s="54"/>
-      <c r="V39" s="54"/>
-      <c r="W39" s="54"/>
-      <c r="X39" s="54"/>
-      <c r="Y39" s="54"/>
-      <c r="Z39" s="54"/>
-      <c r="AA39" s="54"/>
-      <c r="AB39" s="54"/>
-      <c r="AC39" s="54"/>
-      <c r="AD39" s="54"/>
-      <c r="AE39" s="54"/>
-      <c r="AF39" s="54"/>
-      <c r="AG39" s="54"/>
-      <c r="AH39" s="54"/>
-      <c r="AI39" s="54"/>
-      <c r="AJ39" s="54"/>
-      <c r="AK39" s="54"/>
-      <c r="AL39" s="54"/>
-      <c r="AM39" s="54"/>
-      <c r="AN39" s="54"/>
-      <c r="AO39" s="54"/>
-      <c r="AP39" s="54"/>
-      <c r="AQ39" s="54"/>
-      <c r="AR39" s="54"/>
-      <c r="AS39" s="54"/>
-      <c r="AT39" s="54"/>
-      <c r="AU39" s="54"/>
-      <c r="AV39" s="54"/>
-      <c r="AW39" s="54"/>
-      <c r="AX39" s="54"/>
-      <c r="AY39" s="54"/>
-      <c r="AZ39" s="54"/>
-      <c r="BA39" s="54"/>
-      <c r="BB39" s="54"/>
-      <c r="BC39" s="54"/>
-      <c r="BD39" s="54"/>
-      <c r="BE39" s="54"/>
-      <c r="BF39" s="54"/>
-      <c r="BG39" s="54"/>
-      <c r="BH39" s="54"/>
-      <c r="BI39" s="54"/>
-      <c r="BJ39" s="54"/>
-      <c r="BK39" s="54"/>
-      <c r="BL39" s="54"/>
-      <c r="BM39" s="54"/>
-      <c r="BN39" s="54"/>
-    </row>
-    <row r="40" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="54"/>
-      <c r="C40" s="54"/>
-      <c r="D40" s="54"/>
-      <c r="E40" s="55"/>
-      <c r="F40" s="54"/>
-      <c r="G40" s="54"/>
-      <c r="H40" s="54"/>
-      <c r="I40" s="54"/>
-      <c r="J40" s="54"/>
-      <c r="K40" s="54"/>
-      <c r="L40" s="54"/>
-      <c r="M40" s="54"/>
-      <c r="N40" s="54"/>
-      <c r="O40" s="54"/>
-      <c r="P40" s="54"/>
-      <c r="Q40" s="54"/>
-      <c r="R40" s="54"/>
-      <c r="S40" s="54"/>
-      <c r="T40" s="54"/>
-      <c r="U40" s="54"/>
-      <c r="V40" s="54"/>
-      <c r="W40" s="54"/>
-      <c r="X40" s="54"/>
-      <c r="Y40" s="54"/>
-      <c r="Z40" s="54"/>
-      <c r="AA40" s="54"/>
-      <c r="AB40" s="54"/>
-      <c r="AC40" s="54"/>
-      <c r="AD40" s="54"/>
-      <c r="AE40" s="54"/>
-      <c r="AF40" s="54"/>
-      <c r="AG40" s="54"/>
-      <c r="AH40" s="54"/>
-      <c r="AI40" s="54"/>
-      <c r="AJ40" s="54"/>
-      <c r="AK40" s="54"/>
-      <c r="AL40" s="54"/>
-      <c r="AM40" s="54"/>
-      <c r="AN40" s="54"/>
-      <c r="AO40" s="54"/>
-      <c r="AP40" s="54"/>
-      <c r="AQ40" s="54"/>
-      <c r="AR40" s="54"/>
-      <c r="AS40" s="54"/>
-      <c r="AT40" s="54"/>
-      <c r="AU40" s="54"/>
-      <c r="AV40" s="54"/>
-      <c r="AW40" s="54"/>
-      <c r="AX40" s="54"/>
-      <c r="AY40" s="54"/>
-      <c r="AZ40" s="54"/>
-      <c r="BA40" s="54"/>
-      <c r="BB40" s="54"/>
-      <c r="BC40" s="54"/>
-      <c r="BD40" s="54"/>
-      <c r="BE40" s="54"/>
-      <c r="BF40" s="54"/>
-      <c r="BG40" s="54"/>
-      <c r="BH40" s="54"/>
-      <c r="BI40" s="54"/>
-      <c r="BJ40" s="54"/>
-      <c r="BK40" s="54"/>
-      <c r="BL40" s="54"/>
-      <c r="BM40" s="54"/>
-      <c r="BN40" s="54"/>
-    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C2:D2"/>
@@ -7263,7 +7024,7 @@
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="C4:D4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D30:D32 D6:D24">
+  <conditionalFormatting sqref="D27:D29 D6:D23">
     <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -7277,12 +7038,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H30:BK32 H8:BK24">
+  <conditionalFormatting sqref="H27:BK29 H8:BK23">
     <cfRule type="expression" dxfId="2" priority="78">
       <formula>H$5&lt;=Aujourd’hui</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H30:BK32 H7:BK24">
+  <conditionalFormatting sqref="H27:BK29 H7:BK23">
     <cfRule type="expression" dxfId="1" priority="11" stopIfTrue="1">
       <formula>AND(H$5&gt;=$E7+1,H$5&lt;=$E7+$F7-2)</formula>
     </cfRule>
@@ -7352,7 +7113,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D30:D32 D6:D24</xm:sqref>
+          <xm:sqref>D27:D29 D6:D23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="2" id="{6C427F2E-2EF5-46B4-BFA6-7C68148277AC}">
@@ -7374,7 +7135,7 @@
           <xm:sqref>F4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="103" id="{628A03C6-EE71-4B44-A6BA-69DC45906EA6}">
+          <x14:cfRule type="iconSet" priority="111" id="{628A03C6-EE71-4B44-A6BA-69DC45906EA6}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -7390,7 +7151,7 @@
               <x14:cfIcon iconSet="3Signs" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>H30:BK32 H7:BK24</xm:sqref>
+          <xm:sqref>H27:BK29 H7:BK23</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>